<commit_message>
Updated work distribution table (excel) to current formula in mm_v2.
</commit_message>
<xml_diff>
--- a/Assignment2/parallelmm_taskcheck.xlsx
+++ b/Assignment2/parallelmm_taskcheck.xlsx
@@ -1,22 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
-  <workbookPr defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26405"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="9015"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="18200" windowHeight="9020"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="11">
   <si>
     <t>tid</t>
   </si>
@@ -72,7 +77,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -80,12 +85,122 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -387,15 +502,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H12"/>
+  <dimension ref="A1:K12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+    <sheetView tabSelected="1" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="200" workbookViewId="0">
+      <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11">
       <c r="A1" t="s">
         <v>5</v>
       </c>
@@ -415,7 +530,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11">
       <c r="A2">
         <v>1024</v>
       </c>
@@ -426,204 +541,377 @@
         <v>1024</v>
       </c>
       <c r="E2">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="G2">
         <f>E2/2</f>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H2">
         <f>E2/G2</f>
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B4" t="s">
+    <row r="3" spans="1:11" ht="15" thickBot="1"/>
+    <row r="4" spans="1:11" ht="15" thickBot="1">
+      <c r="A4" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" s="8" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>0</v>
-      </c>
-      <c r="B5">
-        <f>INT(A5/$H$2)*INT($A$2/$G$2)</f>
-        <v>0</v>
-      </c>
-      <c r="C5">
-        <f>INT(A5/$H$2+1)*INT($A$2/$G$2)</f>
-        <v>256</v>
-      </c>
-      <c r="D5">
-        <f>INT(A5/$G$2)*INT($B$2/$H$2)</f>
-        <v>0</v>
-      </c>
-      <c r="E5">
-        <f>INT(A5/$G$2+1)*INT($B$2/$H$2)</f>
-        <v>512</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6">
+      <c r="G4" t="s">
+        <v>0</v>
+      </c>
+      <c r="H4" t="s">
         <v>1</v>
       </c>
-      <c r="B6">
-        <f t="shared" ref="B6:B12" si="0">INT(A6/$H$2)*INT($A$2/$G$2)</f>
-        <v>0</v>
-      </c>
-      <c r="C6">
-        <f t="shared" ref="C6:C12" si="1">INT(A6/$H$2+1)*INT($A$2/$G$2)</f>
-        <v>256</v>
-      </c>
-      <c r="D6">
-        <f t="shared" ref="D6:D12" si="2">INT(A6/$G$2)*INT($B$2/$H$2)</f>
-        <v>0</v>
-      </c>
-      <c r="E6">
-        <f t="shared" ref="E6:E12" si="3">INT(A6/$G$2+1)*INT($B$2/$H$2)</f>
-        <v>512</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7">
+      <c r="I4" t="s">
         <v>2</v>
       </c>
-      <c r="B7">
+      <c r="J4" t="s">
+        <v>3</v>
+      </c>
+      <c r="K4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11">
+      <c r="A5" s="3">
+        <v>0</v>
+      </c>
+      <c r="B5" s="5">
+        <f>MOD(INT(A5/$H$2)*INT($A$2/$G$2),$A$2)</f>
+        <v>0</v>
+      </c>
+      <c r="C5" s="5">
+        <f>((MOD(INT(A5/$H$2+1)*INT($A$2/$G$2),$A$2)))</f>
+        <v>512</v>
+      </c>
+      <c r="D5" s="5">
+        <f>MOD(INT(MOD(A5,$G$2))*INT($B$2/$H$2),$B$2)</f>
+        <v>0</v>
+      </c>
+      <c r="E5" s="6">
+        <f>MOD(INT(MOD(A5,$G$2)+1)*INT($B$2/$H$2),$B$2)</f>
+        <v>512</v>
+      </c>
+      <c r="G5">
+        <v>0</v>
+      </c>
+      <c r="H5">
+        <f>B5</f>
+        <v>0</v>
+      </c>
+      <c r="I5">
+        <f>IF(C5=0,$A$2, C5)</f>
+        <v>512</v>
+      </c>
+      <c r="J5">
+        <f>D5</f>
+        <v>0</v>
+      </c>
+      <c r="K5">
+        <f>IF(E5=0,$B$2, E5)</f>
+        <v>512</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11">
+      <c r="A6" s="1">
+        <v>1</v>
+      </c>
+      <c r="B6" s="5">
+        <f t="shared" ref="B6:B12" si="0">MOD(INT(A6/$H$2)*INT($A$2/$G$2),$A$2)</f>
+        <v>0</v>
+      </c>
+      <c r="C6" s="5">
+        <f t="shared" ref="C6:C12" si="1">((MOD(INT(A6/$H$2+1)*INT($A$2/$G$2),$A$2)))</f>
+        <v>512</v>
+      </c>
+      <c r="D6" s="5">
+        <f t="shared" ref="D6:D12" si="2">MOD(INT(MOD(A6,$G$2))*INT($B$2/$H$2),$B$2)</f>
+        <v>512</v>
+      </c>
+      <c r="E6" s="6">
+        <f t="shared" ref="E6:E12" si="3">MOD(INT(MOD(A6,$G$2)+1)*INT($B$2/$H$2),$B$2)</f>
+        <v>0</v>
+      </c>
+      <c r="G6">
+        <v>1</v>
+      </c>
+      <c r="H6">
+        <f t="shared" ref="H6:H12" si="4">B6</f>
+        <v>0</v>
+      </c>
+      <c r="I6">
+        <f t="shared" ref="I6:I12" si="5">IF(C6=0,$A$2, C6)</f>
+        <v>512</v>
+      </c>
+      <c r="J6">
+        <f t="shared" ref="J6:J12" si="6">D6</f>
+        <v>512</v>
+      </c>
+      <c r="K6">
+        <f t="shared" ref="K6:K12" si="7">IF(E6=0,$B$2, E6)</f>
+        <v>1024</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11">
+      <c r="A7" s="1">
+        <v>2</v>
+      </c>
+      <c r="B7" s="5">
         <f t="shared" si="0"/>
-        <v>256</v>
-      </c>
-      <c r="C7">
+        <v>512</v>
+      </c>
+      <c r="C7" s="5">
         <f t="shared" si="1"/>
-        <v>512</v>
-      </c>
-      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="D7" s="5">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="E7">
+      <c r="E7" s="6">
         <f t="shared" si="3"/>
         <v>512</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8">
+      <c r="G7">
+        <v>2</v>
+      </c>
+      <c r="H7">
+        <f t="shared" si="4"/>
+        <v>512</v>
+      </c>
+      <c r="I7">
+        <f t="shared" si="5"/>
+        <v>1024</v>
+      </c>
+      <c r="J7">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="K7">
+        <f t="shared" si="7"/>
+        <v>512</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11">
+      <c r="A8" s="1">
         <v>3</v>
       </c>
-      <c r="B8">
+      <c r="B8" s="5">
         <f t="shared" si="0"/>
-        <v>256</v>
-      </c>
-      <c r="C8">
+        <v>512</v>
+      </c>
+      <c r="C8" s="5">
         <f t="shared" si="1"/>
-        <v>512</v>
-      </c>
-      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="D8" s="5">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="E8">
+        <v>512</v>
+      </c>
+      <c r="E8" s="6">
         <f t="shared" si="3"/>
-        <v>512</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9">
+        <v>0</v>
+      </c>
+      <c r="G8">
+        <v>3</v>
+      </c>
+      <c r="H8">
+        <f t="shared" si="4"/>
+        <v>512</v>
+      </c>
+      <c r="I8">
+        <f t="shared" si="5"/>
+        <v>1024</v>
+      </c>
+      <c r="J8">
+        <f t="shared" si="6"/>
+        <v>512</v>
+      </c>
+      <c r="K8">
+        <f t="shared" si="7"/>
+        <v>1024</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11">
+      <c r="A9" s="1">
         <v>4</v>
       </c>
-      <c r="B9">
+      <c r="B9" s="5">
         <f t="shared" si="0"/>
-        <v>512</v>
-      </c>
-      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="C9" s="5">
         <f t="shared" si="1"/>
-        <v>768</v>
-      </c>
-      <c r="D9">
+        <v>512</v>
+      </c>
+      <c r="D9" s="5">
         <f t="shared" si="2"/>
-        <v>512</v>
-      </c>
-      <c r="E9">
+        <v>0</v>
+      </c>
+      <c r="E9" s="6">
         <f t="shared" si="3"/>
-        <v>1024</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10">
+        <v>512</v>
+      </c>
+      <c r="G9">
+        <v>4</v>
+      </c>
+      <c r="H9">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="I9">
+        <f t="shared" si="5"/>
+        <v>512</v>
+      </c>
+      <c r="J9">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="K9">
+        <f t="shared" si="7"/>
+        <v>512</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11">
+      <c r="A10" s="1">
         <v>5</v>
       </c>
-      <c r="B10">
+      <c r="B10" s="5">
         <f t="shared" si="0"/>
-        <v>512</v>
-      </c>
-      <c r="C10">
+        <v>0</v>
+      </c>
+      <c r="C10" s="5">
         <f t="shared" si="1"/>
-        <v>768</v>
-      </c>
-      <c r="D10">
+        <v>512</v>
+      </c>
+      <c r="D10" s="5">
         <f t="shared" si="2"/>
         <v>512</v>
       </c>
-      <c r="E10">
+      <c r="E10" s="6">
         <f t="shared" si="3"/>
-        <v>1024</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11">
+        <v>0</v>
+      </c>
+      <c r="G10">
+        <v>5</v>
+      </c>
+      <c r="H10">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="I10">
+        <f t="shared" si="5"/>
+        <v>512</v>
+      </c>
+      <c r="J10">
+        <f t="shared" si="6"/>
+        <v>512</v>
+      </c>
+      <c r="K10">
+        <f t="shared" si="7"/>
+        <v>1024</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11">
+      <c r="A11" s="1">
         <v>6</v>
       </c>
-      <c r="B11">
+      <c r="B11" s="5">
         <f t="shared" si="0"/>
-        <v>768</v>
-      </c>
-      <c r="C11">
+        <v>512</v>
+      </c>
+      <c r="C11" s="5">
         <f t="shared" si="1"/>
-        <v>1024</v>
-      </c>
-      <c r="D11">
+        <v>0</v>
+      </c>
+      <c r="D11" s="5">
         <f t="shared" si="2"/>
-        <v>512</v>
-      </c>
-      <c r="E11">
+        <v>0</v>
+      </c>
+      <c r="E11" s="6">
         <f t="shared" si="3"/>
-        <v>1024</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12">
+        <v>512</v>
+      </c>
+      <c r="G11">
+        <v>6</v>
+      </c>
+      <c r="H11">
+        <f t="shared" si="4"/>
+        <v>512</v>
+      </c>
+      <c r="I11">
+        <f t="shared" si="5"/>
+        <v>1024</v>
+      </c>
+      <c r="J11">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="K11">
+        <f t="shared" si="7"/>
+        <v>512</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" ht="15" thickBot="1">
+      <c r="A12" s="2">
         <v>7</v>
       </c>
-      <c r="B12">
+      <c r="B12" s="5">
         <f t="shared" si="0"/>
-        <v>768</v>
-      </c>
-      <c r="C12">
+        <v>512</v>
+      </c>
+      <c r="C12" s="5">
         <f t="shared" si="1"/>
-        <v>1024</v>
-      </c>
-      <c r="D12">
+        <v>0</v>
+      </c>
+      <c r="D12" s="5">
         <f t="shared" si="2"/>
         <v>512</v>
       </c>
-      <c r="E12">
+      <c r="E12" s="6">
         <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="G12">
+        <v>7</v>
+      </c>
+      <c r="H12">
+        <f t="shared" si="4"/>
+        <v>512</v>
+      </c>
+      <c r="I12">
+        <f t="shared" si="5"/>
+        <v>1024</v>
+      </c>
+      <c r="J12">
+        <f t="shared" si="6"/>
+        <v>512</v>
+      </c>
+      <c r="K12">
+        <f t="shared" si="7"/>
         <v>1024</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -633,9 +921,14 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -645,8 +938,13 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>